<commit_message>
Peat types from peat depth raster. Not peat pixels excluded from dry peat volume computation. Working version of SA and GA.
</commit_message>
<xml_diff>
--- a/data/params.xlsx
+++ b/data/params.xlsx
@@ -18,6 +18,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Kadjust for mesic peat. K_Sapric = K_mesic x 0.5
+K_fibric = K_mesic x 2
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -190,12 +216,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -265,7 +291,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
@@ -327,7 +353,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="6" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -345,6 +371,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
block height = 0.2 results
</commit_message>
<xml_diff>
--- a/data/params.xlsx
+++ b/data/params.xlsx
@@ -216,12 +216,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -291,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
plots for yearly wtd
</commit_message>
<xml_diff>
--- a/data/params.xlsx
+++ b/data/params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\dd_winrock\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773E7314-3986-466A-BF05-204AC17C25DD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E79E722-AD6E-484B-AAF3-2A9E942B6567}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,17 +597,17 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0.4</v>
       </c>
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="5">
         <v>1</v>
@@ -675,12 +675,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>

</xml_diff>